<commit_message>
Some changes to the bill of materials
</commit_message>
<xml_diff>
--- a/Bill of Materials/Heimdall Bill of Materials.xlsx
+++ b/Bill of Materials/Heimdall Bill of Materials.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100">
   <si>
     <t>Item #</t>
   </si>
@@ -74,7 +74,7 @@
     <t>Heated bed (200x200mm)</t>
   </si>
   <si>
-    <t>Optional, you can still use the printer without one. You might get more printing area, but might not be able to print with abs.</t>
+    <t>Optional, you can still use the printer without one. You get more printing area, but might not be able to print with abs.</t>
   </si>
   <si>
     <t>Hotend w/ Fan</t>
@@ -89,19 +89,19 @@
     <t>Mechanical Parts</t>
   </si>
   <si>
-    <t>5/16 Stainless Steel Threaded Rod (340mm Long)</t>
+    <t>5/16 - 18 Stainless Steel Threaded Rod (340mm)</t>
   </si>
   <si>
     <t>Home Depot or any hardware store.</t>
   </si>
   <si>
-    <t>Z axis Threaded rod.</t>
-  </si>
-  <si>
-    <t>5/16 Stainless Steel Nuts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You only need one, more just in case. </t>
+    <t xml:space="preserve">Z axis Threaded rod, if you want to use a Metric one, you can use a M8 Stainless Steel threaded rod. </t>
+  </si>
+  <si>
+    <t>5/16 - 18 Stainless Steel Nuts</t>
+  </si>
+  <si>
+    <t>You only need one, more just in case. For Metric, you can use an M8 nut.</t>
   </si>
   <si>
     <t>8mm Hardened Linear Rods X (260mm)</t>
@@ -219,6 +219,9 @@
   </si>
   <si>
     <t>M3 Washers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Washers to get good spacing between parts. </t>
   </si>
   <si>
     <t>M4 Screws (28mm)</t>
@@ -320,9 +323,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -345,9 +348,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -362,7 +372,61 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -376,16 +440,29 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -406,35 +483,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -442,51 +490,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -515,13 +518,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -533,91 +674,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -629,67 +692,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -779,6 +782,36 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -786,6 +819,15 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -813,177 +855,138 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -992,7 +995,7 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
@@ -1016,9 +1019,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1414,8 +1414,8 @@
   <sheetPr/>
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
@@ -1423,7 +1423,7 @@
     <col min="1" max="1" width="11.5238095238095"/>
     <col min="2" max="2" width="44.2285714285714"/>
     <col min="3" max="3" width="16.1047619047619"/>
-    <col min="4" max="4" width="33.247619047619"/>
+    <col min="4" max="4" width="37.1428571428571" customWidth="1"/>
     <col min="5" max="5" width="129.571428571429" customWidth="1"/>
     <col min="6" max="8" width="11.5238095238095"/>
     <col min="9" max="9" width="44.2285714285714"/>
@@ -1457,9 +1457,9 @@
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="H2" s="10"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
+      <c r="H2" s="9"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="3">
@@ -1477,9 +1477,9 @@
       <c r="E3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="10"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
+      <c r="H3" s="9"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="3">
@@ -1497,9 +1497,9 @@
       <c r="E4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="10"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
+      <c r="H4" s="9"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="3">
@@ -1517,9 +1517,9 @@
       <c r="E5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="10"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
+      <c r="H5" s="9"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="3">
@@ -1537,9 +1537,9 @@
       <c r="E6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="10"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
+      <c r="H6" s="9"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="3">
@@ -1557,9 +1557,9 @@
       <c r="E7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="10"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
+      <c r="H7" s="9"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="3">
@@ -1577,9 +1577,9 @@
       <c r="E8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="10"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
+      <c r="H8" s="9"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="3">
@@ -1597,9 +1597,9 @@
       <c r="E9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="10"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
+      <c r="H9" s="9"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="3">
@@ -1617,9 +1617,9 @@
       <c r="E10" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H10" s="10"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11"/>
+      <c r="H10" s="9"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="2" t="s">
@@ -1629,9 +1629,9 @@
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="H11" s="10"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
+      <c r="H11" s="9"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="5">
@@ -1649,9 +1649,9 @@
       <c r="E12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H12" s="10"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
+      <c r="H12" s="9"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="5">
@@ -1669,9 +1669,9 @@
       <c r="E13" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="H13" s="10"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="11"/>
+      <c r="H13" s="9"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="5">
@@ -1689,9 +1689,9 @@
       <c r="E14" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="H14" s="10"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11"/>
+      <c r="H14" s="9"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="5">
@@ -1709,9 +1709,9 @@
       <c r="E15" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="H15" s="10"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
+      <c r="H15" s="9"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="5">
@@ -1729,9 +1729,9 @@
       <c r="E16" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="H16" s="10"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
+      <c r="H16" s="9"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="5">
@@ -1749,9 +1749,9 @@
       <c r="E17" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="H17" s="10"/>
-      <c r="K17" s="11"/>
-      <c r="L17" s="11"/>
+      <c r="H17" s="9"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="5">
@@ -1769,9 +1769,9 @@
       <c r="E18" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="H18" s="10"/>
-      <c r="K18" s="11"/>
-      <c r="L18" s="11"/>
+      <c r="H18" s="9"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="5">
@@ -1789,9 +1789,9 @@
       <c r="E19" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="H19" s="10"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="11"/>
+      <c r="H19" s="9"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
     </row>
     <row r="20" spans="1:12">
       <c r="A20" s="5">
@@ -1809,9 +1809,9 @@
       <c r="E20" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="H20" s="10"/>
-      <c r="K20" s="11"/>
-      <c r="L20" s="11"/>
+      <c r="H20" s="9"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="5">
@@ -1829,9 +1829,9 @@
       <c r="E21" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="H21" s="10"/>
-      <c r="K21" s="11"/>
-      <c r="L21" s="11"/>
+      <c r="H21" s="9"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="5">
@@ -1849,9 +1849,9 @@
       <c r="E22" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="H22" s="10"/>
-      <c r="K22" s="11"/>
-      <c r="L22" s="11"/>
+      <c r="H22" s="9"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="5">
@@ -1869,9 +1869,9 @@
       <c r="E23" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="H23" s="10"/>
-      <c r="K23" s="11"/>
-      <c r="L23" s="11"/>
+      <c r="H23" s="9"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
     </row>
     <row r="24" spans="1:12">
       <c r="A24" s="5">
@@ -1889,9 +1889,9 @@
       <c r="E24" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="H24" s="10"/>
-      <c r="K24" s="11"/>
-      <c r="L24" s="11"/>
+      <c r="H24" s="9"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
     </row>
     <row r="25" spans="1:12">
       <c r="A25" s="5">
@@ -1909,9 +1909,9 @@
       <c r="E25" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="H25" s="10"/>
-      <c r="K25" s="11"/>
-      <c r="L25" s="11"/>
+      <c r="H25" s="9"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="5">
@@ -1929,7 +1929,7 @@
       <c r="E26" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="H26" s="10"/>
+      <c r="H26" s="9"/>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="5">
@@ -1947,7 +1947,7 @@
       <c r="E27" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="H27" s="10"/>
+      <c r="H27" s="9"/>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="5">
@@ -1965,7 +1965,7 @@
       <c r="E28" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H28" s="10"/>
+      <c r="H28" s="9"/>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="2" t="s">
@@ -1975,7 +1975,7 @@
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
-      <c r="H29" s="10"/>
+      <c r="H29" s="9"/>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="6">
@@ -1993,7 +1993,7 @@
       <c r="E30" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="H30" s="10"/>
+      <c r="H30" s="9"/>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="5">
@@ -2011,29 +2011,32 @@
       <c r="E31" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="H31" s="10"/>
+      <c r="H31" s="9"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="8">
+      <c r="A32" s="3">
         <v>28</v>
       </c>
       <c r="B32" t="s">
         <v>67</v>
       </c>
-      <c r="C32" s="8">
+      <c r="C32" s="3">
         <v>120</v>
       </c>
       <c r="D32" t="s">
         <v>63</v>
       </c>
-      <c r="H32" s="10"/>
+      <c r="E32" t="s">
+        <v>68</v>
+      </c>
+      <c r="H32" s="9"/>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="5">
         <v>29</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C33" s="5">
         <v>2</v>
@@ -2042,16 +2045,16 @@
         <v>63</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="H33" s="10"/>
+        <v>70</v>
+      </c>
+      <c r="H33" s="9"/>
     </row>
     <row r="34" spans="1:12">
       <c r="A34" s="3">
         <v>30</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C34" s="5">
         <v>1</v>
@@ -2060,20 +2063,20 @@
         <v>63</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="H34" s="10"/>
-      <c r="I34" s="11"/>
-      <c r="J34" s="10"/>
-      <c r="K34" s="11"/>
-      <c r="L34" s="11"/>
+        <v>72</v>
+      </c>
+      <c r="H34" s="9"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="9"/>
+      <c r="K34" s="10"/>
+      <c r="L34" s="10"/>
     </row>
     <row r="35" spans="1:12">
       <c r="A35" s="3">
         <v>31</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C35" s="5">
         <v>1</v>
@@ -2082,20 +2085,20 @@
         <v>63</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="H35" s="10"/>
-      <c r="I35" s="11"/>
-      <c r="J35" s="10"/>
-      <c r="K35" s="11"/>
-      <c r="L35" s="11"/>
+        <v>72</v>
+      </c>
+      <c r="H35" s="9"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="9"/>
+      <c r="K35" s="10"/>
+      <c r="L35" s="10"/>
     </row>
     <row r="36" spans="1:12">
       <c r="A36" s="5">
         <v>32</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C36" s="5">
         <v>4</v>
@@ -2104,20 +2107,20 @@
         <v>63</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="H36" s="10"/>
-      <c r="I36" s="11"/>
-      <c r="J36" s="10"/>
-      <c r="K36" s="11"/>
-      <c r="L36" s="11"/>
+        <v>75</v>
+      </c>
+      <c r="H36" s="9"/>
+      <c r="I36" s="10"/>
+      <c r="J36" s="9"/>
+      <c r="K36" s="10"/>
+      <c r="L36" s="10"/>
     </row>
     <row r="37" spans="1:12">
       <c r="A37" s="5">
         <v>33</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C37" s="5">
         <v>8</v>
@@ -2126,20 +2129,20 @@
         <v>63</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="H37" s="10"/>
-      <c r="I37" s="11"/>
-      <c r="J37" s="10"/>
-      <c r="K37" s="11"/>
-      <c r="L37" s="11"/>
+        <v>77</v>
+      </c>
+      <c r="H37" s="9"/>
+      <c r="I37" s="10"/>
+      <c r="J37" s="9"/>
+      <c r="K37" s="10"/>
+      <c r="L37" s="10"/>
     </row>
     <row r="38" spans="1:12">
       <c r="A38" s="5">
         <v>34</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C38" s="5">
         <v>8</v>
@@ -2148,20 +2151,20 @@
         <v>63</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="H38" s="10"/>
-      <c r="I38" s="11"/>
-      <c r="J38" s="10"/>
-      <c r="K38" s="11"/>
-      <c r="L38" s="11"/>
+        <v>77</v>
+      </c>
+      <c r="H38" s="9"/>
+      <c r="I38" s="10"/>
+      <c r="J38" s="9"/>
+      <c r="K38" s="10"/>
+      <c r="L38" s="10"/>
     </row>
     <row r="39" spans="1:12">
-      <c r="A39" s="9">
+      <c r="A39" s="8">
         <v>35</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C39" s="5">
         <v>8</v>
@@ -2170,65 +2173,65 @@
         <v>63</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="H39" s="10"/>
-      <c r="I39" s="11"/>
-      <c r="J39" s="10"/>
-      <c r="K39" s="11"/>
-      <c r="L39" s="11"/>
+        <v>80</v>
+      </c>
+      <c r="H39" s="9"/>
+      <c r="I39" s="10"/>
+      <c r="J39" s="9"/>
+      <c r="K39" s="10"/>
+      <c r="L39" s="10"/>
     </row>
     <row r="40" spans="1:12">
       <c r="A40" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
-      <c r="H40" s="10"/>
-      <c r="I40" s="11"/>
-      <c r="J40" s="10"/>
-      <c r="K40" s="11"/>
-      <c r="L40" s="11"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="10"/>
+      <c r="J40" s="9"/>
+      <c r="K40" s="10"/>
+      <c r="L40" s="10"/>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="6">
         <v>36</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C41" s="5">
         <v>1</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="42" spans="1:5">
-      <c r="A42" s="9">
+      <c r="A42" s="8">
         <v>37</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C42" s="5">
         <v>4</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -2240,7 +2243,7 @@
         <v>38</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C44" s="5">
         <v>1</v>
@@ -2249,7 +2252,7 @@
         <v>7</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -2257,7 +2260,7 @@
         <v>39</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C45" s="5">
         <v>1</v>
@@ -2266,7 +2269,7 @@
         <v>7</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -2274,16 +2277,16 @@
         <v>40</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C46" s="5">
         <v>1</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -2291,16 +2294,16 @@
         <v>41</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C47" s="3">
         <v>1</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -2308,7 +2311,7 @@
         <v>42</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C48" s="5">
         <v>1</v>
@@ -2317,11 +2320,11 @@
         <v>25</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="49" spans="1:1">
-      <c r="A49" s="8"/>
+      <c r="A49" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>